<commit_message>
case : update database
</commit_message>
<xml_diff>
--- a/uploads/excelsales.xlsx
+++ b/uploads/excelsales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\first\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A66A12-D9B6-4917-9F44-CBCC06EBD78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AA634E-A0B8-478B-AD80-AA129A851475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date_Sales</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Name_Company</t>
-  </si>
-  <si>
-    <t>FIRSTSTEP</t>
   </si>
 </sst>
 </file>
@@ -393,7 +390,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -421,8 +418,8 @@
       <c r="A2" s="7">
         <v>242644</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" s="2">
+        <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>

</xml_diff>